<commit_message>
draft with data in shiny
</commit_message>
<xml_diff>
--- a/Data/00_Raw_Data/06_pg_pendler/Pendler_pro_Gemeinde_Jahr_2000.xlsx
+++ b/Data/00_Raw_Data/06_pg_pendler/Pendler_pro_Gemeinde_Jahr_2000.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reto\OneDrive - ETHZ\Dokumente\ETH\Bauland\Bauland\Data\00_Raw_Data\06_pg_pendler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{FE3722E6-CDB3-45A6-BA6A-CF6618C86F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F0519F65-5A1F-4E07-A174-159748835BB7}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{FE3722E6-CDB3-45A6-BA6A-CF6618C86F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5D4FAEE0-E3FE-4E53-9068-80ABB741D7A0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15825" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -17407,10 +17407,10 @@
     <t>name</t>
   </si>
   <si>
-    <t>pendlersaldo_person</t>
-  </si>
-  <si>
-    <t>pendlersaldo_percent_worker</t>
+    <t>mob_pendler_saldo</t>
+  </si>
+  <si>
+    <t>mob_ant_pendler_saldo</t>
   </si>
 </sst>
 </file>
@@ -17420,11 +17420,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -17462,7 +17468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -17476,6 +17482,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17783,10 +17790,10 @@
   <dimension ref="A1:D2909"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C2042" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2906" sqref="A2906:D2906"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -17804,10 +17811,10 @@
       <c r="B1" t="s">
         <v>5794</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>5795</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>5796</v>
       </c>
     </row>

</xml_diff>